<commit_message>
gerber and production files updated
</commit_message>
<xml_diff>
--- a/gerber/BOM_RHS_3.xlsx
+++ b/gerber/BOM_RHS_3.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="122">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -73,6 +73,78 @@
     <t xml:space="preserve">9p</t>
   </si>
   <si>
+    <t xml:space="preserve">C14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">330Âµ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_SMD:CP_Elec_6.3x5.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4u7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitor_SMD:C_0402_1005Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22 C27 C21 C20 C19 C18 C17 C16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1525</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1547</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25 C28 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3p3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1565</t>
+  </si>
+  <si>
     <t xml:space="preserve">C4 C5 C6 </t>
   </si>
   <si>
@@ -124,6 +196,18 @@
     <t xml:space="preserve">libraries:CC1101_Module</t>
   </si>
   <si>
+    <t xml:space="preserve">IC3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC1101_Chip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_DFN_QFN:QFN-20-1EP_4x4mm_P0.5mm_EP2.5x2.5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29953</t>
+  </si>
+  <si>
     <t xml:space="preserve">J1 </t>
   </si>
   <si>
@@ -142,6 +226,36 @@
     <t xml:space="preserve">Connector_Pin:Pin_D1.0mm_L10.0mm</t>
   </si>
   <si>
+    <t xml:space="preserve">JP1 JP2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumper_NO_Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jumper:SolderJumper-2_P1.3mm_Bridged_Pad1.0x1.5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1 L2 L5 L6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12nH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductor_SMD:L_0402_1005Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24563</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L3 L4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18nH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24562</t>
+  </si>
+  <si>
     <t xml:space="preserve">P4 </t>
   </si>
   <si>
@@ -175,7 +289,19 @@
     <t xml:space="preserve">Connector_PinHeader_2.54mm:PinHeader_2x05_P2.54mm_Vertical</t>
   </si>
   <si>
-    <t xml:space="preserve">R1 </t>
+    <t xml:space="preserve">Q1 Q2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si2305CDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C37577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 R9 R10 </t>
   </si>
   <si>
     <t xml:space="preserve">10k</t>
@@ -205,6 +331,18 @@
     <t xml:space="preserve">C17514</t>
   </si>
   <si>
+    <t xml:space="preserve">R8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">56k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistor_SMD:R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25796</t>
+  </si>
+  <si>
     <t xml:space="preserve">SW1 </t>
   </si>
   <si>
@@ -226,7 +364,19 @@
     <t xml:space="preserve">TLE4913</t>
   </si>
   <si>
-    <t xml:space="preserve">Package_TO_SOT_SMD:SOT-23</t>
+    <t xml:space="preserve">C126654</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resonator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oscillator:Oscillator_SMD_EuroQuartz_XO32-4Pin_3.2x2.5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C91747</t>
   </si>
   <si>
     <t xml:space="preserve">Y1 </t>
@@ -245,12 +395,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -264,6 +413,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
     </font>
@@ -310,8 +465,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,24 +491,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -432,15 +591,12 @@
         <v>17</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
         <v>19</v>
       </c>
     </row>
@@ -466,116 +622,134 @@
         <v>24</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="0" t="s">
         <v>47</v>
       </c>
     </row>
@@ -590,6 +764,9 @@
         <v>49</v>
       </c>
       <c r="D16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>50</v>
       </c>
     </row>
@@ -615,15 +792,12 @@
         <v>55</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="0" t="s">
         <v>57</v>
       </c>
     </row>
@@ -632,72 +806,309 @@
         <v>58</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>